<commit_message>
Add source folder configuration for POW Sequencer
- Updated VBA module with SelectSourceFolder and CheckSourceFiles macros
- Added Configurazione sheet to Excel template for source path setting
- System now shows file modification dates before generating MDB
- Created Sorgenti folder for storing modified MDB files from Powin-PC2

Workflow: Modify in Powin-PC2 -> Save to Sorgenti -> Generate combined MDB
</commit_message>
<xml_diff>
--- a/POW_Sequencer_Template.xlsx
+++ b/POW_Sequencer_Template.xlsx
@@ -8,7 +8,8 @@
   </bookViews>
   <sheets>
     <sheet name="Sequenza" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Istruzioni" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Configurazione" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Istruzioni" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -18,7 +19,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -31,8 +32,11 @@
       <color rgb="00FFFFFF"/>
       <sz val="12"/>
     </font>
+    <font>
+      <b val="1"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill/>
     </fill>
@@ -43,6 +47,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="004472C4"/>
         <bgColor rgb="004472C4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00E2EFDA"/>
+        <bgColor rgb="00E2EFDA"/>
       </patternFill>
     </fill>
   </fills>
@@ -64,12 +74,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -554,7 +567,93 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A25"/>
+  <dimension ref="A1:C7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="20" customWidth="1" min="1" max="1"/>
+    <col width="50" customWidth="1" min="2" max="2"/>
+    <col width="45" customWidth="1" min="3" max="3"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="3" t="inlineStr">
+        <is>
+          <t>Impostazione</t>
+        </is>
+      </c>
+      <c r="B1" s="3" t="inlineStr">
+        <is>
+          <t>Valore</t>
+        </is>
+      </c>
+      <c r="C1" s="3" t="inlineStr">
+        <is>
+          <t>Descrizione</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="4" t="inlineStr">
+        <is>
+          <t>Cartella Sorgenti</t>
+        </is>
+      </c>
+      <c r="B2" s="4" t="inlineStr">
+        <is>
+          <t>default</t>
+        </is>
+      </c>
+      <c r="C2" s="4" t="inlineStr">
+        <is>
+          <t>Percorso dove salvare i file MDB da Powin-PC2</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="5" t="inlineStr">
+        <is>
+          <t>NOTE:</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>- 'default' = usa la cartella 'Sorgenti' nella stessa directory del file Excel</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>- Esegui la macro 'SelectSourceFolder' per selezionare una cartella diversa</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>- Esegui la macro 'CheckSourceFiles' per verificare lo stato dei file</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -568,7 +667,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>POW PROGRAM SEQUENCER</t>
+          <t>POW PROGRAM SEQUENCER - GUIDA</t>
         </is>
       </c>
     </row>
@@ -578,149 +677,281 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>COME USARE:</t>
+          <t>CONFIGURAZIONE INIZIALE:</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>1. Nel foglio 'Sequenza', inserisci i numeri dei programmi nella colonna A</t>
+          <t>1. Crea una cartella 'Sorgenti' nella stessa directory del file Excel</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2. L'ordine delle righe determina la sequenza di esecuzione</t>
+          <t>2. Oppure usa la macro 'SelectSourceFolder' per scegliere una cartella diversa</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>3. Salva il file come .xlsm (con macro abilitate)</t>
+          <t>3. Salva i file MDB da Powin-PC2 nella cartella Sorgenti:</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>4. Importa il modulo VBA 'POW_Sequencer_VBA.bas'</t>
+          <t xml:space="preserve">   - 30IGNIT.mdb</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>5. Esegui la macro 'GenerateMDB'</t>
+          <t xml:space="preserve">   - 31NOWELD.mdb</t>
         </is>
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="inlineStr"/>
+      <c r="A9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   - 32WELD.mdb</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>PROGRAMMI DISPONIBILI:</t>
+          <t xml:space="preserve">   - 33DWNSLP.mdb</t>
         </is>
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  30 = IGNIT (Accensione) - 12 funzioni</t>
-        </is>
-      </c>
+      <c r="A11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t xml:space="preserve">  31 = NOWELD (No saldatura) - 39 funzioni</t>
+          <t>FLUSSO DI LAVORO:</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t xml:space="preserve">  32 = WELD (Saldatura) - 49 funzioni</t>
+          <t>1. Modifica i parametri in Powin-PC2</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t xml:space="preserve">  33 = DWNSLP (Downslope) - 49 funzioni</t>
+          <t>2. Esporta/Salva il programma modificato come file MDB</t>
         </is>
       </c>
     </row>
     <row r="15">
-      <c r="A15" t="inlineStr"/>
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>3. Copia il file MDB nella cartella Sorgenti</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>ESEMPIO:</t>
+          <t>4. Apri questo Excel e imposta la sequenza</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Se inserisci: 30, 33, 31</t>
+          <t>5. Esegui 'GenerateMDB' per creare il file combinato</t>
         </is>
       </c>
     </row>
     <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>Il programma MDB conterrà:</t>
-        </is>
-      </c>
+      <c r="A18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t xml:space="preserve">  - Prima tutte le funzioni di 30IGNIT (righe 1-11)</t>
+          <t>COME USARE:</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t xml:space="preserve">  - Poi tutte le funzioni di 33DWNSLP (righe 12-59)</t>
+          <t>1. Nel foglio 'Sequenza', inserisci i numeri nella colonna A</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t xml:space="preserve">  - Infine tutte le funzioni di 31NOWELD (righe 60-97)</t>
+          <t>2. L'ordine delle righe determina la sequenza di esecuzione</t>
         </is>
       </c>
     </row>
     <row r="22">
-      <c r="A22" t="inlineStr"/>
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>3. Salva il file come .xlsm (con macro)</t>
+        </is>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>ALTERNATIVA PYTHON:</t>
+          <t>4. Importa il modulo VBA 'POW_Sequencer_VBA.bas'</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Puoi anche usare lo script pow_sequencer.py:</t>
+          <t>5. Esegui la macro 'GenerateMDB'</t>
         </is>
       </c>
     </row>
     <row r="25">
-      <c r="A25" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  python pow_sequencer.py --interactive</t>
+      <c r="A25" t="inlineStr"/>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>PROGRAMMI DISPONIBILI:</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  30 = IGNIT (Accensione) - 12 funzioni</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  31 = NOWELD (No saldatura) - 39 funzioni</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  32 = WELD (Saldatura) - 49 funzioni</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  33 = DWNSLP (Downslope) - 49 funzioni</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr"/>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>MACRO DISPONIBILI:</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  GenerateMDB       - Genera il file MDB dalla sequenza</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  SelectSourceFolder - Seleziona la cartella sorgenti</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  CheckSourceFiles   - Verifica stato dei file sorgente</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  ClearSequence      - Pulisce la sequenza</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  AddDefaultSequence - Aggiunge sequenza 30-31-32-33</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  ShowHelp           - Mostra la guida</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr"/>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>ESEMPIO:</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>Se inserisci: 30, 32, 33</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>Il programma MDB finale conterra:</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  - Prima tutte le funzioni di 30IGNIT (righe 1-11)</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  - Poi tutte le funzioni di 32WELD (righe 12-59)</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  - Infine tutte le funzioni di 33DWNSLP (righe 60-107)</t>
         </is>
       </c>
     </row>

</xml_diff>